<commit_message>
Automatisacion de jefes de carrera campos y sombreado de horas b
</commit_message>
<xml_diff>
--- a/static/src/Plantilla_pie_reducido_2cm.xlsx
+++ b/static/src/Plantilla_pie_reducido_2cm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chapa\Desktop\tecnologico\static\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CACB7B-0960-4941-8C93-789E28BF2285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D9B7F6-4271-42C2-BCFC-91AC8C31B6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>“2024. Año del Bicentenario de la Erección del Estado Libre y Soberano de México”</t>
   </si>
@@ -191,18 +191,6 @@
   </si>
   <si>
     <t>Vo. Bo</t>
-  </si>
-  <si>
-    <t>DRA C.CLAUDIA PÉREZ MARTÍNEZ</t>
-  </si>
-  <si>
-    <t>DIRECTORA GENERAL</t>
-  </si>
-  <si>
-    <t>ENCARGADA DEL DESPACHO DE DIRECCIÓN ACADÉMICA</t>
-  </si>
-  <si>
-    <t>LCDA. BLANCA ESTELA SÁNCHEZ HERNÁNDEZ</t>
   </si>
 </sst>
 </file>
@@ -213,7 +201,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -293,13 +281,6 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="6"/>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -576,7 +557,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="108">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -689,10 +670,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,39 +688,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -751,6 +706,40 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -771,51 +760,80 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1166,8 +1184,8 @@
   </sheetPr>
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A36" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J4"/>
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A35" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1191,150 +1209,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="84"/>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="74"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="75" t="s">
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="66"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="64"/>
     </row>
     <row r="8" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="75" t="s">
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="75" t="s">
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="61"/>
     </row>
     <row r="9" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="88"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="66"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
     </row>
     <row r="10" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="76" t="s">
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="76" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="74"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="77"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
       <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1362,18 +1380,18 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="74"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
@@ -1529,18 +1547,18 @@
       <c r="K23" s="17"/>
     </row>
     <row r="24" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
     </row>
     <row r="25" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
@@ -1694,18 +1712,18 @@
       <c r="K34" s="27"/>
     </row>
     <row r="35" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
     </row>
     <row r="36" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
@@ -1768,10 +1786,10 @@
     </row>
     <row r="39" spans="1:17" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="36"/>
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="80"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="37"/>
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
@@ -1785,24 +1803,24 @@
       <c r="B40" s="40"/>
       <c r="C40" s="41"/>
       <c r="D40" s="38"/>
-      <c r="E40" s="81" t="s">
+      <c r="E40" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="69"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="80"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="83"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="81"/>
     </row>
     <row r="41" spans="1:17" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36"/>
       <c r="B41" s="40"/>
       <c r="C41" s="41"/>
       <c r="D41" s="38"/>
-      <c r="E41" s="81" t="s">
+      <c r="E41" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="69"/>
+      <c r="F41" s="55"/>
       <c r="G41" s="42"/>
       <c r="H41" s="38"/>
       <c r="I41" s="38"/>
@@ -1819,231 +1837,246 @@
       <c r="J42" s="44"/>
       <c r="K42" s="45"/>
     </row>
-    <row r="43" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="91"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="92" t="s">
+    <row r="43" spans="1:17" s="43" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="106"/>
+      <c r="B43" s="107"/>
+      <c r="C43" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="72" t="s">
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="H43" s="73"/>
-      <c r="I43" s="73"/>
-      <c r="J43" s="74"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="58"/>
       <c r="K43" s="45"/>
     </row>
-    <row r="44" spans="1:17" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="46"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="60"/>
+    <row r="44" spans="1:17" s="43" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="102"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="71"/>
       <c r="K44" s="45"/>
     </row>
-    <row r="45" spans="1:17" s="43" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="54"/>
-      <c r="B45"/>
-      <c r="C45" s="93" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="94"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="95"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="63"/>
+    <row r="45" spans="1:17" s="43" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="104"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="100"/>
+      <c r="E45" s="100"/>
+      <c r="F45" s="101"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="88"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="89"/>
       <c r="K45" s="45"/>
     </row>
-    <row r="46" spans="1:17" s="43" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="67"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="96" t="s">
-        <v>36</v>
-      </c>
+    <row r="46" spans="1:17" s="43" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="91"/>
+      <c r="B46" s="92"/>
+      <c r="C46" s="96"/>
       <c r="D46" s="97"/>
       <c r="E46" s="97"/>
       <c r="F46" s="98"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="65"/>
-      <c r="I46" s="65"/>
-      <c r="J46" s="66"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="64"/>
       <c r="K46" s="45"/>
     </row>
     <row r="47" spans="1:17" ht="1.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="50"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
-      <c r="P47" s="51"/>
-      <c r="Q47" s="51"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="P47" s="49"/>
+      <c r="Q47" s="49"/>
     </row>
     <row r="48" spans="1:17" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="68"/>
-      <c r="B48" s="69"/>
-      <c r="C48" s="99" t="s">
+      <c r="A48" s="93"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="70"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="69"/>
-      <c r="J48" s="69"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="94"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="69"/>
-      <c r="B49" s="69"/>
-      <c r="C49" s="100"/>
-      <c r="D49" s="100"/>
-      <c r="E49" s="100"/>
-      <c r="F49" s="100"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="69"/>
-      <c r="J49" s="69"/>
+      <c r="A49" s="55"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="55"/>
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="69"/>
-      <c r="B50" s="69"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="69"/>
+      <c r="A50" s="55"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="95"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="95"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="53"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
       <c r="K51" s="3"/>
     </row>
     <row r="52" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="53"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="53"/>
+      <c r="A52" s="51"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="83"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C53" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="57"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="84"/>
-      <c r="B54" s="84"/>
-      <c r="C54" s="84"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
-      <c r="F54" s="84"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="84"/>
-      <c r="I54" s="84"/>
-      <c r="J54" s="84"/>
+      <c r="A54" s="53"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="84"/>
-      <c r="B55" s="84"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="84"/>
-      <c r="G55" s="84"/>
-      <c r="H55" s="84"/>
-      <c r="I55" s="84"/>
-      <c r="J55" s="84"/>
+      <c r="A55" s="53"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="84"/>
-      <c r="B56" s="84"/>
-      <c r="C56" s="84"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="84"/>
-      <c r="F56" s="84"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="84"/>
-      <c r="I56" s="84"/>
-      <c r="J56" s="84"/>
+      <c r="A56" s="53"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="84"/>
-      <c r="B57" s="84"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="84"/>
-      <c r="G57" s="84"/>
-      <c r="H57" s="84"/>
-      <c r="I57" s="84"/>
-      <c r="J57" s="84"/>
+      <c r="A57" s="53"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="53"/>
       <c r="K57" s="3"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="84"/>
-      <c r="B58" s="84"/>
-      <c r="C58" s="84"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="84"/>
-      <c r="F58" s="84"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="84"/>
-      <c r="I58" s="84"/>
-      <c r="J58" s="84"/>
+      <c r="A58" s="53"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="53"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="84"/>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84"/>
-      <c r="D59" s="84"/>
-      <c r="E59" s="84"/>
-      <c r="F59" s="84"/>
-      <c r="G59" s="84"/>
-      <c r="H59" s="84"/>
-      <c r="I59" s="84"/>
-      <c r="J59" s="84"/>
+      <c r="A59" s="53"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="39">
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="G44:J46"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A48:B50"/>
+    <mergeCell ref="C48:F50"/>
+    <mergeCell ref="G48:J50"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="E41:F41"/>
     <mergeCell ref="A54:J59"/>
     <mergeCell ref="A1:J3"/>
     <mergeCell ref="A4:J4"/>
@@ -2060,27 +2093,6 @@
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C43:F43"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="G44:J46"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A48:B50"/>
-    <mergeCell ref="C48:F50"/>
-    <mergeCell ref="G48:J50"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="C45:F45"/>
   </mergeCells>
   <conditionalFormatting sqref="E15:J22">
     <cfRule type="endsWith" dxfId="3" priority="2" operator="endsWith" text=".">

</xml_diff>